<commit_message>
atualizado 09 11 22
pagina menu  50%
</commit_message>
<xml_diff>
--- a/Banco de dados.xlsx
+++ b/Banco de dados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -637,6 +637,114 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Celso</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>31 985615649</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Rua : Salvia 162</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bruno Marcelino </t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>31 9 85467898</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Femenino</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rua :  do pau comeu </t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Breno Josefino </t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>31 9 87658906</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rua ; Faca na caveira </t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Lindeia</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>234234234</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Femenino</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>23432423423423</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>